<commit_message>
TXN Update & Refactor
</commit_message>
<xml_diff>
--- a/Stock-Analysis/AAPL/AAPL.xlsx
+++ b/Stock-Analysis/AAPL/AAPL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bcb0b6f0298eff0f/Investing-Repo/Stock-Analysis/AAPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{FCD0D65F-5E57-4337-A2DB-36D296810CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B72C4A35-85FD-4354-BADE-BC503C9A9ECB}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{FCD0D65F-5E57-4337-A2DB-36D296810CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80E0823B-9744-4E3F-8BB5-ADC210CF2EF1}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="720" activeTab="1" xr2:uid="{9825DF3D-1B58-4C24-A60D-565D808A20BC}"/>
+    <workbookView xWindow="3060" yWindow="1230" windowWidth="21600" windowHeight="11295" tabRatio="720" activeTab="3" xr2:uid="{9825DF3D-1B58-4C24-A60D-565D808A20BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Aesop" sheetId="4" r:id="rId1"/>
@@ -3320,7 +3320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8FA1C0-125F-4E09-8416-0C3BFF7D9B7A}">
   <dimension ref="B2:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S3" sqref="S3:S32"/>
     </sheetView>
   </sheetViews>
@@ -5301,8 +5301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD77939E-B893-4A61-818C-43CD02673FE9}">
   <dimension ref="B2:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6581,8 +6581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77BD8A2-DF5A-465F-B8A0-1AAAA5C7FD7E}">
   <dimension ref="B2:R32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D32" sqref="D29:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6596,7 +6596,7 @@
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>

</xml_diff>